<commit_message>
3 small tests run
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="18240" windowHeight="7380"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="18240" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>HTTP</t>
   </si>
@@ -47,7 +47,13 @@
     <t>fileName</t>
   </si>
   <si>
-    <t>testLinews35</t>
+    <t>test.txt</t>
+  </si>
+  <si>
+    <t>test2.txt</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -63,12 +69,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -122,11 +146,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,7 +473,7 @@
   <dimension ref="A2:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,166 +513,294 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>35</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>351</v>
+      </c>
+      <c r="F3" s="4">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="E4" s="3">
+        <v>352</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="E5" s="3">
+        <v>354</v>
+      </c>
+      <c r="F5" s="4">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="3">
+        <v>353</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="3">
+        <v>353</v>
+      </c>
+      <c r="F7" s="4">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>324</v>
+      </c>
+      <c r="F8" s="6">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5">
+        <v>325</v>
+      </c>
+      <c r="F9" s="6">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5">
+        <v>324</v>
+      </c>
+      <c r="F10" s="6">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
+        <v>321</v>
+      </c>
+      <c r="F11" s="6">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5">
+        <v>322</v>
+      </c>
+      <c r="F12" s="6">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="A13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>89</v>
+      </c>
+      <c r="F13" s="8">
+        <v>10</v>
+      </c>
+      <c r="G13" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7">
+        <v>88</v>
+      </c>
+      <c r="F14" s="8">
+        <v>10</v>
+      </c>
+      <c r="G14" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7">
+        <v>88</v>
+      </c>
+      <c r="F15" s="8">
+        <v>10</v>
+      </c>
+      <c r="G15" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7">
+        <v>89</v>
+      </c>
+      <c r="F16" s="8">
+        <v>10</v>
+      </c>
+      <c r="G16" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7">
+        <v>90</v>
+      </c>
+      <c r="F17" s="8">
+        <v>10</v>
+      </c>
+      <c r="G17" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>